<commit_message>
ajout force stabilisation dans repère scapula dans OutputFile
</commit_message>
<xml_diff>
--- a/Application/Validation/EpauleFDK/Output/Resultats FDK/Valeurs Forces de stabilisation.xlsx
+++ b/Application/Validation/EpauleFDK/Output/Resultats FDK/Valeurs Forces de stabilisation.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mes Documents\ETS\Projet de recherche\EpauleFDK\Application\Validation\EpauleFDK\Output\Resultats FDK\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dan\Documents\Gitkraken\EpauleFDK\Application\Validation\EpauleFDK\Output\Resultats FDK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F1D898A-795F-46B1-AFEF-9959657C5981}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCEC3471-C20B-484F-A993-BC6643549B97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{C3F7F2A6-C0DB-41C8-9B1C-2A92373F98FF}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C3F7F2A6-C0DB-41C8-9B1C-2A92373F98FF}"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
-    <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
+    <sheet name="Force stabilisation" sheetId="1" r:id="rId1"/>
+    <sheet name="RoM" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -945,8 +945,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DD7A112-F69A-4DA1-8C4E-6359FAB7A5B9}">
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1180,7 +1180,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5EE7BC2-D1B2-4300-9EC2-E9CBBB4ACA4E}">
   <dimension ref="A1:U68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I72" sqref="I72"/>
     </sheetView>
   </sheetViews>

</xml_diff>